<commit_message>
Generated pie chart of refactoring operations clustered by class.
</commit_message>
<xml_diff>
--- a/Python/IssueRefactoringDocCalculator/issue_refactoring_doc_text_patterns.csv.xlsx
+++ b/Python/IssueRefactoringDocCalculator/issue_refactoring_doc_text_patterns.csv.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SmartSHARK\GitSmartSHARKfilePathconflict\SmartSHARKRepo\Python\IssueRefactoringDocCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8C3E83-2DDD-48DD-A90F-AA766E87418F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B20B674-E1F0-40A5-93C7-05A8716794E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="textual_patterns_treemap" sheetId="4" r:id="rId1"/>
     <sheet name="sunburst" sheetId="5" r:id="rId2"/>
     <sheet name="pie_chart" sheetId="6" r:id="rId3"/>
     <sheet name="issue_title_refactoring_doc_tex" sheetId="1" r:id="rId4"/>
-    <sheet name="ref_ops_clustered_pie" sheetId="9" r:id="rId5"/>
+    <sheet name="ref_ops_pie" sheetId="10" r:id="rId5"/>
     <sheet name="ref_ops_clustered_by_class" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
@@ -2364,13 +2364,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Refactoring Operations</a:t>
+              <a:t>Refactoring Operations Clustered by Class</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Clustered by Class</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2431,7 +2426,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-910D-42B3-B334-289617F4E265}"/>
+                <c16:uniqueId val="{00000001-C33E-4B63-ABE5-571D286C4783}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2455,7 +2450,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-910D-42B3-B334-289617F4E265}"/>
+                <c16:uniqueId val="{00000003-C33E-4B63-ABE5-571D286C4783}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2479,7 +2474,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-910D-42B3-B334-289617F4E265}"/>
+                <c16:uniqueId val="{00000005-C33E-4B63-ABE5-571D286C4783}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2503,7 +2498,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-910D-42B3-B334-289617F4E265}"/>
+                <c16:uniqueId val="{00000007-C33E-4B63-ABE5-571D286C4783}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2527,91 +2522,11 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-910D-42B3-B334-289617F4E265}"/>
+                <c16:uniqueId val="{00000009-C33E-4B63-ABE5-571D286C4783}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="ctr"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-910D-42B3-B334-289617F4E265}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="ctr"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-910D-42B3-B334-289617F4E265}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="ctr"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-910D-42B3-B334-289617F4E265}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="ctr"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-910D-42B3-B334-289617F4E265}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="ctr"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-910D-42B3-B334-289617F4E265}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
             <c:spPr>
               <a:pattFill prst="pct75">
                 <a:fgClr>
@@ -2659,7 +2574,7 @@
             </c:txPr>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
+            <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="1"/>
@@ -2712,26 +2627,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>18028</c:v>
+                  <c:v>18078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14026</c:v>
+                  <c:v>14080</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1418</c:v>
+                  <c:v>1432</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8675</c:v>
+                  <c:v>8695</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3215</c:v>
+                  <c:v>3231</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-910D-42B3-B334-289617F4E265}"/>
+              <c16:uniqueId val="{0000000A-C33E-4B63-ABE5-571D286C4783}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5437,7 +5352,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{7CF6B2EA-EBB2-4938-9730-DC6812712D51}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{8BBD98B6-4146-4ACE-ADB7-2B03FA3A826B}">
   <sheetPr/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" workbookViewId="0" zoomToFit="1"/>
@@ -5517,7 +5432,7 @@
         <cdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42C4D24C-DB66-12DD-6F69-B8B166E8252C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B55DFF05-C16D-1684-5F07-C1EACA2159D6}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -5628,7 +5543,7 @@
         <cdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{230C47B5-0ED3-69EF-8252-9FEA7CCE8CF1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1947AC2-133C-6395-1E93-300BAD4BE180}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -5712,7 +5627,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BB20452-718D-653F-355F-44348611233F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72BEB4C2-3F64-D2F6-F445-464D3738252C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7233,7 +7148,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7257,19 +7172,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>18028</v>
+        <v>18078</v>
       </c>
       <c r="B2">
-        <v>14026</v>
+        <v>14080</v>
       </c>
       <c r="C2">
-        <v>1418</v>
+        <v>1432</v>
       </c>
       <c r="D2">
-        <v>8675</v>
+        <v>8695</v>
       </c>
       <c r="E2">
-        <v>3215</v>
+        <v>3231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>